<commit_message>
correction binding group 8441e9368a4991ec6607e0ebd1cf8b6ab17af0d2
</commit_message>
<xml_diff>
--- a/ig/sd-creation-de-codeSystems-StudyPopulation-RegulationCode-ReglementationPrecision/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/sd-creation-de-codeSystems-StudyPopulation-RegulationCode-ReglementationPrecision/StructureDefinition-eclaire-researchstudy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="457">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-10-13T11:58:38+00:00</t>
+    <t>2023-10-14T08:48:02+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -916,25 +916,25 @@
     <t>Codes categorizing the type of study such as investigational vs. observational, type of blinding, type of randomization, safety vs. efficacy, etc.</t>
   </si>
   <si>
+    <t>https://interop.esante.gouv.fr/ig/fhir/eclaire/ValueSet/eclaire-category-vs</t>
+  </si>
+  <si>
+    <t>InterventionalStudyProtocolVersion; InterventionalStudyProtocol.allocationCode; InterventionalStudyProtocol.blindedRoleCode; InterventionalStudyProtocol.blindingSchemaCode; InterventionalStudyProtocol.controlTypeCode</t>
+  </si>
+  <si>
+    <t>Study Type; Primary Purpose; Interventional Model; Masking; Allocation; study Classification; Observational Study Model; Time Perspective; Biospecimen Retention</t>
+  </si>
+  <si>
+    <t>ResearchStudy.focus</t>
+  </si>
+  <si>
+    <t>Drugs, devices, etc. under study</t>
+  </si>
+  <si>
+    <t>The medication(s), food(s), therapy(ies), device(s) or other concerns or interventions that the study is seeking to gain more information about.</t>
+  </si>
+  <si>
     <t>example</t>
-  </si>
-  <si>
-    <t>Codes that describe the type of research study.  E.g. Study phase, Interventional/Observational, blinding type, etc.</t>
-  </si>
-  <si>
-    <t>InterventionalStudyProtocolVersion; InterventionalStudyProtocol.allocationCode; InterventionalStudyProtocol.blindedRoleCode; InterventionalStudyProtocol.blindingSchemaCode; InterventionalStudyProtocol.controlTypeCode</t>
-  </si>
-  <si>
-    <t>Study Type; Primary Purpose; Interventional Model; Masking; Allocation; study Classification; Observational Study Model; Time Perspective; Biospecimen Retention</t>
-  </si>
-  <si>
-    <t>ResearchStudy.focus</t>
-  </si>
-  <si>
-    <t>Drugs, devices, etc. under study</t>
-  </si>
-  <si>
-    <t>The medication(s), food(s), therapy(ies), device(s) or other concerns or interventions that the study is seeking to gain more information about.</t>
   </si>
   <si>
     <t>Codes for medications, devices and other interventions.</t>
@@ -1779,7 +1779,7 @@
     <col min="22" max="22" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="10.53125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="106.69140625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="98.375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="71.046875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="11.08203125" customWidth="true" bestFit="true"/>
@@ -6553,13 +6553,11 @@
         <v>37</v>
       </c>
       <c r="X41" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="Y41" s="2"/>
+      <c r="Z41" t="s" s="2">
         <v>287</v>
-      </c>
-      <c r="Y41" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="Z41" t="s" s="2">
-        <v>37</v>
       </c>
       <c r="AA41" t="s" s="2">
         <v>37</v>
@@ -6592,7 +6590,7 @@
         <v>60</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>276</v>
@@ -6601,7 +6599,7 @@
         <v>277</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>37</v>
@@ -6609,10 +6607,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6638,10 +6636,10 @@
         <v>178</v>
       </c>
       <c r="L42" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="M42" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>293</v>
       </c>
       <c r="N42" t="s" s="2">
         <v>272</v>
@@ -6670,7 +6668,7 @@
         <v>37</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="Y42" t="s" s="2">
         <v>294</v>
@@ -6694,7 +6692,7 @@
         <v>37</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>35</v>
@@ -6787,7 +6785,7 @@
         <v>37</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="Y43" t="s" s="2">
         <v>301</v>
@@ -7717,7 +7715,7 @@
         <v>37</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="Y51" t="s" s="2">
         <v>341</v>
@@ -8653,7 +8651,7 @@
         <v>37</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="Y59" t="s" s="2">
         <v>400</v>

</xml_diff>